<commit_message>
Se actualiza el script de indicadores de rendimientos, queda pendiente una mejor maquetacion y enviarlo por correo
</commit_message>
<xml_diff>
--- a/DB/reporte_turnos.xlsx
+++ b/DB/reporte_turnos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\turnero\DB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0411114F-5173-47E5-9B0B-ED3CE5AD6319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6D395E1-3987-4CBA-BDDE-AE8027113B8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Usuario ID</t>
   </si>
@@ -46,10 +46,22 @@
     <t>laura</t>
   </si>
   <si>
-    <t>2024-08-26</t>
+    <t>2024-09-09</t>
   </si>
   <si>
     <t>rocio</t>
+  </si>
+  <si>
+    <t>Hora Pico Global</t>
+  </si>
+  <si>
+    <t>Turnos en Hora Pico Global</t>
+  </si>
+  <si>
+    <t>Total Clientes Atendidos</t>
+  </si>
+  <si>
+    <t>Tiempo Promedio de Espera (min)</t>
   </si>
 </sst>
 </file>
@@ -391,21 +403,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5546875" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="24.5546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.44140625" customWidth="1"/>
-    <col min="7" max="7" width="19" customWidth="1"/>
+    <col min="1" max="1" width="48.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.88671875" customWidth="1"/>
+    <col min="3" max="3" width="17.5546875" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="21.109375" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
@@ -442,16 +453,16 @@
         <v>8</v>
       </c>
       <c r="D2">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="E2">
-        <v>1360.8333</v>
+        <v>1182.6429000000001</v>
       </c>
       <c r="F2">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="G2">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
@@ -465,16 +476,53 @@
         <v>8</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="E3">
-        <v>30</v>
+        <v>1443.6667</v>
       </c>
       <c r="F3">
+        <v>14</v>
+      </c>
+      <c r="G3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>1303.1153999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="G3">
-        <v>2</v>
+      <c r="B6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>1303.1153999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>